<commit_message>
Last change before draft
</commit_message>
<xml_diff>
--- a/Other Files/PastResults.xlsx
+++ b/Other Files/PastResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\011445\Documents\GitHub\TLTBO\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277C80C3-BECD-4C1E-89D0-1FF182F109E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8C4351-460C-4280-9913-9F8F2912879F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Statistics WW" sheetId="5" r:id="rId5"/>
     <sheet name="Statistics 5M" sheetId="6" r:id="rId6"/>
     <sheet name="Template" sheetId="7" r:id="rId7"/>
+    <sheet name="1804" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="165">
   <si>
     <t>Thank you for taking the time to view the past results and statistics. I hope that these will help you to succeed more in the future, and you learn from them.</t>
   </si>
@@ -5000,8 +5001,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AL1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5048,15 +5049,15 @@
     </row>
     <row r="5" spans="2:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="36" t="str">
-        <f>Template!C2</f>
+        <f>'1804'!C2</f>
         <v>Insert Date Here</v>
       </c>
       <c r="C5" s="3">
-        <f>COUNT(Template!B3:B30)</f>
+        <f>COUNT('1804'!B3:B30)</f>
         <v>16</v>
       </c>
       <c r="D5" s="3">
-        <f>MAX(Template!L3:L5)</f>
+        <f>MAX('1804'!L3:L5)</f>
         <v>7</v>
       </c>
       <c r="E5" s="3">
@@ -5064,7 +5065,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="3">
-        <f>MIN(Template!L3:L5)</f>
+        <f>MIN('1804'!L3:L5)</f>
         <v>4</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -5955,7 +5956,7 @@
         <v>55</v>
       </c>
       <c r="Q29" s="44">
-        <f>Template!R3</f>
+        <f>'1804'!R3</f>
         <v>1</v>
       </c>
       <c r="R29" s="29">
@@ -5963,7 +5964,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="27">
-        <f>Template!S3</f>
+        <f>'1804'!S3</f>
         <v>0</v>
       </c>
       <c r="T29" s="28">
@@ -5971,7 +5972,7 @@
         <v>0</v>
       </c>
       <c r="U29" s="27">
-        <f>Template!T3</f>
+        <f>'1804'!T3</f>
         <v>1</v>
       </c>
       <c r="V29" s="28">
@@ -5979,7 +5980,7 @@
         <v>1</v>
       </c>
       <c r="W29" s="27">
-        <f>Template!U3</f>
+        <f>'1804'!U3</f>
         <v>0</v>
       </c>
       <c r="X29" s="28">
@@ -5996,7 +5997,7 @@
         <v>59</v>
       </c>
       <c r="Q30" s="44">
-        <f>Template!R4</f>
+        <f>'1804'!R4</f>
         <v>1</v>
       </c>
       <c r="R30" s="29">
@@ -6004,7 +6005,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="27">
-        <f>Template!S4</f>
+        <f>'1804'!S4</f>
         <v>0</v>
       </c>
       <c r="T30" s="28">
@@ -6012,7 +6013,7 @@
         <v>0</v>
       </c>
       <c r="U30" s="27">
-        <f>Template!T4</f>
+        <f>'1804'!T4</f>
         <v>1</v>
       </c>
       <c r="V30" s="28">
@@ -6020,7 +6021,7 @@
         <v>1</v>
       </c>
       <c r="W30" s="27">
-        <f>Template!U4</f>
+        <f>'1804'!U4</f>
         <v>0</v>
       </c>
       <c r="X30" s="28">
@@ -6037,7 +6038,7 @@
         <v>62</v>
       </c>
       <c r="Q31" s="44">
-        <f>Template!R5</f>
+        <f>'1804'!R5</f>
         <v>2</v>
       </c>
       <c r="R31" s="29">
@@ -6045,7 +6046,7 @@
         <v>2</v>
       </c>
       <c r="S31" s="27">
-        <f>Template!S5</f>
+        <f>'1804'!S5</f>
         <v>0</v>
       </c>
       <c r="T31" s="28">
@@ -6053,7 +6054,7 @@
         <v>0</v>
       </c>
       <c r="U31" s="27">
-        <f>Template!T5</f>
+        <f>'1804'!T5</f>
         <v>0</v>
       </c>
       <c r="V31" s="28">
@@ -6061,7 +6062,7 @@
         <v>0</v>
       </c>
       <c r="W31" s="27">
-        <f>Template!U5</f>
+        <f>'1804'!U5</f>
         <v>1</v>
       </c>
       <c r="X31" s="28">
@@ -6078,7 +6079,7 @@
         <v>65</v>
       </c>
       <c r="Q32" s="44">
-        <f>Template!R6</f>
+        <f>'1804'!R6</f>
         <v>2</v>
       </c>
       <c r="R32" s="29">
@@ -6086,7 +6087,7 @@
         <v>2</v>
       </c>
       <c r="S32" s="27">
-        <f>Template!S6</f>
+        <f>'1804'!S6</f>
         <v>0</v>
       </c>
       <c r="T32" s="28">
@@ -6094,7 +6095,7 @@
         <v>0</v>
       </c>
       <c r="U32" s="27">
-        <f>Template!T6</f>
+        <f>'1804'!T6</f>
         <v>0</v>
       </c>
       <c r="V32" s="28">
@@ -6102,7 +6103,7 @@
         <v>0</v>
       </c>
       <c r="W32" s="27">
-        <f>Template!U6</f>
+        <f>'1804'!U6</f>
         <v>1</v>
       </c>
       <c r="X32" s="28">
@@ -6118,7 +6119,7 @@
         <v>68</v>
       </c>
       <c r="Q33" s="44">
-        <f>Template!R7</f>
+        <f>'1804'!R7</f>
         <v>1</v>
       </c>
       <c r="R33" s="29">
@@ -6126,7 +6127,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="27">
-        <f>Template!S7</f>
+        <f>'1804'!S7</f>
         <v>0</v>
       </c>
       <c r="T33" s="28">
@@ -6134,7 +6135,7 @@
         <v>0</v>
       </c>
       <c r="U33" s="27">
-        <f>Template!T7</f>
+        <f>'1804'!T7</f>
         <v>1</v>
       </c>
       <c r="V33" s="28">
@@ -6142,7 +6143,7 @@
         <v>1</v>
       </c>
       <c r="W33" s="27">
-        <f>Template!U7</f>
+        <f>'1804'!U7</f>
         <v>0</v>
       </c>
       <c r="X33" s="28">
@@ -6158,7 +6159,7 @@
         <v>71</v>
       </c>
       <c r="Q34" s="44">
-        <f>Template!R8</f>
+        <f>'1804'!R8</f>
         <v>1</v>
       </c>
       <c r="R34" s="29">
@@ -6166,7 +6167,7 @@
         <v>1</v>
       </c>
       <c r="S34" s="27">
-        <f>Template!S8</f>
+        <f>'1804'!S8</f>
         <v>0</v>
       </c>
       <c r="T34" s="28">
@@ -6174,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="U34" s="27">
-        <f>Template!T8</f>
+        <f>'1804'!T8</f>
         <v>1</v>
       </c>
       <c r="V34" s="28">
@@ -6182,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="W34" s="27">
-        <f>Template!U8</f>
+        <f>'1804'!U8</f>
         <v>0</v>
       </c>
       <c r="X34" s="28">
@@ -6198,7 +6199,7 @@
         <v>75</v>
       </c>
       <c r="Q35" s="44">
-        <f>Template!R9</f>
+        <f>'1804'!R9</f>
         <v>2</v>
       </c>
       <c r="R35" s="29">
@@ -6206,7 +6207,7 @@
         <v>2</v>
       </c>
       <c r="S35" s="27">
-        <f>Template!S9</f>
+        <f>'1804'!S9</f>
         <v>0</v>
       </c>
       <c r="T35" s="28">
@@ -6214,7 +6215,7 @@
         <v>0</v>
       </c>
       <c r="U35" s="27">
-        <f>Template!T9</f>
+        <f>'1804'!T9</f>
         <v>0</v>
       </c>
       <c r="V35" s="28">
@@ -6222,7 +6223,7 @@
         <v>0</v>
       </c>
       <c r="W35" s="27">
-        <f>Template!U9</f>
+        <f>'1804'!U9</f>
         <v>1</v>
       </c>
       <c r="X35" s="28">
@@ -6238,7 +6239,7 @@
         <v>78</v>
       </c>
       <c r="Q36" s="44">
-        <f>Template!R10</f>
+        <f>'1804'!R10</f>
         <v>1</v>
       </c>
       <c r="R36" s="29">
@@ -6246,7 +6247,7 @@
         <v>1</v>
       </c>
       <c r="S36" s="27">
-        <f>Template!S10</f>
+        <f>'1804'!S10</f>
         <v>1</v>
       </c>
       <c r="T36" s="28">
@@ -6254,7 +6255,7 @@
         <v>1</v>
       </c>
       <c r="U36" s="27">
-        <f>Template!T10</f>
+        <f>'1804'!T10</f>
         <v>0</v>
       </c>
       <c r="V36" s="28">
@@ -6262,7 +6263,7 @@
         <v>0</v>
       </c>
       <c r="W36" s="27">
-        <f>Template!U10</f>
+        <f>'1804'!U10</f>
         <v>0</v>
       </c>
       <c r="X36" s="28">
@@ -6278,7 +6279,7 @@
         <v>80</v>
       </c>
       <c r="Q37" s="44">
-        <f>Template!R11</f>
+        <f>'1804'!R11</f>
         <v>2</v>
       </c>
       <c r="R37" s="29">
@@ -6286,7 +6287,7 @@
         <v>2</v>
       </c>
       <c r="S37" s="27">
-        <f>Template!S11</f>
+        <f>'1804'!S11</f>
         <v>0</v>
       </c>
       <c r="T37" s="28">
@@ -6294,7 +6295,7 @@
         <v>0</v>
       </c>
       <c r="U37" s="27">
-        <f>Template!T11</f>
+        <f>'1804'!T11</f>
         <v>2</v>
       </c>
       <c r="V37" s="28">
@@ -6302,7 +6303,7 @@
         <v>2</v>
       </c>
       <c r="W37" s="27">
-        <f>Template!U11</f>
+        <f>'1804'!U11</f>
         <v>0</v>
       </c>
       <c r="X37" s="28">
@@ -6318,7 +6319,7 @@
         <v>81</v>
       </c>
       <c r="Q38" s="44">
-        <f>Template!R12</f>
+        <f>'1804'!R12</f>
         <v>1</v>
       </c>
       <c r="R38" s="29">
@@ -6326,7 +6327,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="27">
-        <f>Template!S12</f>
+        <f>'1804'!S12</f>
         <v>0</v>
       </c>
       <c r="T38" s="28">
@@ -6334,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="U38" s="27">
-        <f>Template!T12</f>
+        <f>'1804'!T12</f>
         <v>1</v>
       </c>
       <c r="V38" s="28">
@@ -6342,7 +6343,7 @@
         <v>1</v>
       </c>
       <c r="W38" s="27">
-        <f>Template!U12</f>
+        <f>'1804'!U12</f>
         <v>0</v>
       </c>
       <c r="X38" s="28">
@@ -6355,7 +6356,7 @@
         <v>82</v>
       </c>
       <c r="Q39" s="44">
-        <f>Template!R13</f>
+        <f>'1804'!R13</f>
         <v>2</v>
       </c>
       <c r="R39" s="29">
@@ -6363,7 +6364,7 @@
         <v>2</v>
       </c>
       <c r="S39" s="27">
-        <f>Template!S13</f>
+        <f>'1804'!S13</f>
         <v>0</v>
       </c>
       <c r="T39" s="28">
@@ -6371,7 +6372,7 @@
         <v>0</v>
       </c>
       <c r="U39" s="27">
-        <f>Template!T13</f>
+        <f>'1804'!T13</f>
         <v>0</v>
       </c>
       <c r="V39" s="28">
@@ -6379,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="W39" s="27">
-        <f>Template!U13</f>
+        <f>'1804'!U13</f>
         <v>1</v>
       </c>
       <c r="X39" s="28">
@@ -6394,7 +6395,7 @@
         <v>83</v>
       </c>
       <c r="Q40" s="44">
-        <f>Template!R14</f>
+        <f>'1804'!R14</f>
         <v>1</v>
       </c>
       <c r="R40" s="29">
@@ -6402,7 +6403,7 @@
         <v>1</v>
       </c>
       <c r="S40" s="27">
-        <f>Template!S14</f>
+        <f>'1804'!S14</f>
         <v>1</v>
       </c>
       <c r="T40" s="28">
@@ -6410,7 +6411,7 @@
         <v>1</v>
       </c>
       <c r="U40" s="27">
-        <f>Template!T14</f>
+        <f>'1804'!T14</f>
         <v>0</v>
       </c>
       <c r="V40" s="28">
@@ -6418,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="W40" s="27">
-        <f>Template!U14</f>
+        <f>'1804'!U14</f>
         <v>0</v>
       </c>
       <c r="X40" s="28">
@@ -6431,7 +6432,7 @@
         <v>86</v>
       </c>
       <c r="Q41" s="44">
-        <f>Template!R15</f>
+        <f>'1804'!R15</f>
         <v>1</v>
       </c>
       <c r="R41" s="29">
@@ -6439,7 +6440,7 @@
         <v>1</v>
       </c>
       <c r="S41" s="27">
-        <f>Template!S15</f>
+        <f>'1804'!S15</f>
         <v>1</v>
       </c>
       <c r="T41" s="28">
@@ -6447,7 +6448,7 @@
         <v>1</v>
       </c>
       <c r="U41" s="27">
-        <f>Template!T15</f>
+        <f>'1804'!T15</f>
         <v>0</v>
       </c>
       <c r="V41" s="28">
@@ -6455,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="W41" s="27">
-        <f>Template!U15</f>
+        <f>'1804'!U15</f>
         <v>0</v>
       </c>
       <c r="X41" s="28">
@@ -6468,7 +6469,7 @@
         <v>87</v>
       </c>
       <c r="Q42" s="44">
-        <f>Template!R16</f>
+        <f>'1804'!R16</f>
         <v>2</v>
       </c>
       <c r="R42" s="29">
@@ -6476,7 +6477,7 @@
         <v>2</v>
       </c>
       <c r="S42" s="27">
-        <f>Template!S16</f>
+        <f>'1804'!S16</f>
         <v>0</v>
       </c>
       <c r="T42" s="28">
@@ -6484,7 +6485,7 @@
         <v>0</v>
       </c>
       <c r="U42" s="27">
-        <f>Template!T16</f>
+        <f>'1804'!T16</f>
         <v>0</v>
       </c>
       <c r="V42" s="28">
@@ -6492,7 +6493,7 @@
         <v>0</v>
       </c>
       <c r="W42" s="27">
-        <f>Template!U16</f>
+        <f>'1804'!U16</f>
         <v>1</v>
       </c>
       <c r="X42" s="28">
@@ -6505,7 +6506,7 @@
         <v>88</v>
       </c>
       <c r="Q43" s="44">
-        <f>Template!R17</f>
+        <f>'1804'!R17</f>
         <v>1</v>
       </c>
       <c r="R43" s="29">
@@ -6513,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="S43" s="27">
-        <f>Template!S17</f>
+        <f>'1804'!S17</f>
         <v>1</v>
       </c>
       <c r="T43" s="28">
@@ -6521,7 +6522,7 @@
         <v>1</v>
       </c>
       <c r="U43" s="27">
-        <f>Template!T17</f>
+        <f>'1804'!T17</f>
         <v>0</v>
       </c>
       <c r="V43" s="28">
@@ -6529,7 +6530,7 @@
         <v>0</v>
       </c>
       <c r="W43" s="27">
-        <f>Template!U17</f>
+        <f>'1804'!U17</f>
         <v>0</v>
       </c>
       <c r="X43" s="28">
@@ -7614,7 +7615,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4:W4"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7703,21 +7704,33 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="4" t="str">
+        <f>'1804'!C2</f>
+        <v>Insert Date Here</v>
+      </c>
+      <c r="B4" s="16">
+        <f>'1804'!L3</f>
+        <v>4</v>
+      </c>
+      <c r="C4" s="16">
+        <f>'1804'!M3</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="16">
+        <f>'1804'!O3</f>
+        <v>1</v>
+      </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:H4" si="0">SUM(B4:B30)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="60"/>
@@ -7726,21 +7739,21 @@
       <c r="N4" s="17"/>
       <c r="O4" s="60"/>
       <c r="Q4" s="17">
-        <f>COUNTIF(Template!W4:W26,"LG/WW")</f>
+        <f>COUNTIF('1804'!W4:W26,"LG/WW")</f>
         <v>2</v>
       </c>
       <c r="R4" s="17">
-        <f>COUNTIF(Template!X4:X26,"WW/LG")</f>
+        <f>COUNTIF('1804'!X4:X26,"WW/LG")</f>
         <v>2</v>
       </c>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="V4" s="17">
-        <f>COUNTIF(Template!W4:W26,"LG/5M")</f>
+        <f>COUNTIF('1804'!W4:W26,"LG/5M")</f>
         <v>2</v>
       </c>
       <c r="W4" s="17">
-        <f>COUNTIF(Template!Y4:Y26,"5M/LG")</f>
+        <f>COUNTIF('1804'!Y4:Y26,"5M/LG")</f>
         <v>4</v>
       </c>
       <c r="X4" s="17"/>
@@ -9295,8 +9308,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4:W4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9386,21 +9399,33 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="4" t="str">
+        <f>'1804'!C2</f>
+        <v>Insert Date Here</v>
+      </c>
+      <c r="B4" s="16">
+        <f>'1804'!L5</f>
+        <v>5</v>
+      </c>
+      <c r="C4" s="16">
+        <f>'1804'!M5</f>
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f>'1804'!O5</f>
+        <v>2</v>
+      </c>
       <c r="F4" s="24">
         <f t="shared" ref="F4:H4" si="0">SUM(B4:B30)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G4" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="60"/>
@@ -9409,21 +9434,21 @@
       <c r="N4" s="17"/>
       <c r="O4" s="60"/>
       <c r="Q4" s="17">
-        <f>COUNTIF(Template!X4:X26,"WW/LG")</f>
+        <f>COUNTIF('1804'!X4:X26,"WW/LG")</f>
         <v>2</v>
       </c>
       <c r="R4" s="17">
-        <f>COUNTIF(Template!W4:W26,"LG/WW")</f>
+        <f>COUNTIF('1804'!W4:W26,"LG/WW")</f>
         <v>2</v>
       </c>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="V4" s="17">
-        <f>COUNTIF(Template!X4:X26,"WW/5M")</f>
+        <f>COUNTIF('1804'!X4:X26,"WW/5M")</f>
         <v>3</v>
       </c>
       <c r="W4" s="17">
-        <f>COUNTIF(Template!Y4:Y26,"5M/WW")</f>
+        <f>COUNTIF('1804'!Y4:Y26,"5M/WW")</f>
         <v>3</v>
       </c>
       <c r="X4" s="17"/>
@@ -10978,8 +11003,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -11069,21 +11094,33 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="4" t="str">
+        <f>'1804'!C2</f>
+        <v>Insert Date Here</v>
+      </c>
+      <c r="B4" s="16">
+        <f>'1804'!L4</f>
+        <v>7</v>
+      </c>
+      <c r="C4" s="16">
+        <f>'1804'!M4</f>
+        <v>5</v>
+      </c>
+      <c r="D4" s="16">
+        <f>'1804'!O4</f>
+        <v>3</v>
+      </c>
       <c r="F4" s="24">
         <f t="shared" ref="F4:H4" si="0">SUM(B4:B30)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G4" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="60"/>
@@ -11092,21 +11129,21 @@
       <c r="N4" s="17"/>
       <c r="O4" s="60"/>
       <c r="Q4" s="17">
-        <f>COUNTIF(Template!Y4:Y26,"5M/LG")</f>
+        <f>COUNTIF('1804'!Y4:Y26,"5M/LG")</f>
         <v>4</v>
       </c>
       <c r="R4" s="17">
-        <f>COUNTIF(Template!W4:W26,"LG/WW")</f>
+        <f>COUNTIF('1804'!W4:W26,"LG/WW")</f>
         <v>2</v>
       </c>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="V4" s="17">
-        <f>COUNTIF(Template!Y4:Y26,"5M/WW")</f>
+        <f>COUNTIF('1804'!Y4:Y26,"5M/WW")</f>
         <v>3</v>
       </c>
       <c r="W4" s="17">
-        <f>COUNTIF(Template!X4:X26,"WW/5M")</f>
+        <f>COUNTIF('1804'!X4:X26,"WW/5M")</f>
         <v>3</v>
       </c>
       <c r="X4" s="17"/>
@@ -12662,7 +12699,7 @@
   <dimension ref="B1:Y1000"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -12745,26 +12782,26 @@
       </c>
       <c r="L3" s="1">
         <f>COUNTIF(C3:C30, "Loose Gooses")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1">
         <f>COUNTIF(D3:D30, "Loose Gooses")</f>
-        <v>6</v>
-      </c>
-      <c r="N3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="23" t="e">
         <f t="shared" ref="N3:N5" si="0">L3/(L3+M3)</f>
-        <v>0.4</v>
-      </c>
-      <c r="O3" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O3" s="1" t="e">
         <f>IF(AND(N3&gt;N4, N3&gt;N5), 3, IF(OR(N3&gt;N4, N3&gt;N5), 2, 1))</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="R3" s="19">
         <f t="shared" ref="R3:R17" si="1">COUNTIF($E$3:$E$27, Q3)+U3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="20">
         <f t="shared" ref="S3:S17" si="2">COUNTIFS($E$3:$E$27, $Q3,$F$3:$F$27,"Finish")</f>
@@ -12772,7 +12809,7 @@
       </c>
       <c r="T3" s="20">
         <f t="shared" ref="T3:T17" si="3">COUNTIFS($E$3:$E$27, $Q3,$F$3:$F$27,"Midrange")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" s="20">
         <f t="shared" ref="U3:U17" si="4">COUNTIFS($E$3:$E$27, $Q3,$F$3:$F$27,"Three Pointer")</f>
@@ -12790,52 +12827,38 @@
       </c>
     </row>
     <row r="4" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="59">
-        <v>1</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="59">
-        <v>1</v>
-      </c>
-      <c r="H4" s="59">
-        <v>1</v>
-      </c>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
       <c r="K4" s="1" t="s">
         <v>139</v>
       </c>
       <c r="L4" s="1">
         <f>COUNTIF(C3:C30, "5 Musketeers")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
         <f>COUNTIF(D3:D30, "5 Musketeers")</f>
-        <v>5</v>
-      </c>
-      <c r="N4" s="23">
+        <v>0</v>
+      </c>
+      <c r="N4" s="23" t="e">
         <f t="shared" si="0"/>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="O4" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O4" s="1" t="e">
         <f>IF(AND(N4&gt;N3, N4&gt;N5), 3, IF(OR(N4&gt;N3, N4&gt;N5), 2, 1))</f>
-        <v>3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="R4" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="20">
         <f t="shared" si="2"/>
@@ -12843,7 +12866,7 @@
       </c>
       <c r="T4" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="20">
         <f t="shared" si="4"/>
@@ -12851,7 +12874,7 @@
       </c>
       <c r="W4" s="1" t="str">
         <f>IF(AND(C4="Loose Gooses",D4="Wet Willies"),"LG/WW", IF(AND(C4="Loose Gooses",D4="5 Musketeers"),"LG/5M", ""))</f>
-        <v>LG/5M</v>
+        <v/>
       </c>
       <c r="X4" s="1" t="str">
         <f>IF(AND(C4="Wet Willies",D4="Loose Gooses"),"WW/LG", IF(AND(C4="Wet Willies",D4="5 Musketeers"),"WW/5M", ""))</f>
@@ -12863,52 +12886,38 @@
       </c>
     </row>
     <row r="5" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="59">
-        <v>2</v>
-      </c>
-      <c r="C5" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" s="59">
-        <v>2</v>
-      </c>
-      <c r="H5" s="59">
-        <v>1</v>
-      </c>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
       <c r="K5" s="1" t="s">
         <v>138</v>
       </c>
       <c r="L5" s="1">
         <f>COUNTIF(C3:C30, "Wet Willies")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
         <f>COUNTIF(D3:D30, "Wet Willies")</f>
-        <v>5</v>
-      </c>
-      <c r="N5" s="23">
+        <v>0</v>
+      </c>
+      <c r="N5" s="23" t="e">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="O5" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" s="1" t="e">
         <f>IF(AND(N5&gt;N4, N5&gt;N3), 3, IF(OR(N5&gt;N4, N5&gt;N3), 2, 1))</f>
-        <v>2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="R5" s="19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S5" s="20">
         <f t="shared" si="2"/>
@@ -12920,11 +12929,11 @@
       </c>
       <c r="U5" s="20">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" s="24" t="str">
         <f t="shared" ref="W5:W28" si="5">IF(AND(C5="Loose Gooses",D5="Wet Willies"),"LG/WW", IF(AND(C5="Loose Gooses",D5="5 Musketeers"),"LG/5M", ""))</f>
-        <v>LG/WW</v>
+        <v/>
       </c>
       <c r="X5" s="24" t="str">
         <f t="shared" ref="X5:X28" si="6">IF(AND(C5="Wet Willies",D5="Loose Gooses"),"WW/LG", IF(AND(C5="Wet Willies",D5="5 Musketeers"),"WW/5M", ""))</f>
@@ -12936,33 +12945,19 @@
       </c>
     </row>
     <row r="6" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="59">
-        <v>3</v>
-      </c>
-      <c r="C6" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="G6" s="59">
-        <v>3</v>
-      </c>
-      <c r="H6" s="59">
-        <v>2</v>
-      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
       <c r="Q6" s="3" t="s">
         <v>44</v>
       </c>
       <c r="R6" s="19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S6" s="20">
         <f t="shared" si="2"/>
@@ -12974,11 +12969,11 @@
       </c>
       <c r="U6" s="20">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="24" t="str">
         <f t="shared" si="5"/>
-        <v>LG/5M</v>
+        <v/>
       </c>
       <c r="X6" s="24" t="str">
         <f t="shared" si="6"/>
@@ -12990,33 +12985,19 @@
       </c>
     </row>
     <row r="7" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="59">
-        <v>4</v>
-      </c>
-      <c r="C7" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="59">
-        <v>4</v>
-      </c>
-      <c r="H7" s="59">
-        <v>2</v>
-      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
       <c r="Q7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="R7" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="20">
         <f t="shared" si="2"/>
@@ -13024,7 +13005,7 @@
       </c>
       <c r="T7" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="20">
         <f t="shared" si="4"/>
@@ -13032,7 +13013,7 @@
       </c>
       <c r="W7" s="24" t="str">
         <f t="shared" si="5"/>
-        <v>LG/WW</v>
+        <v/>
       </c>
       <c r="X7" s="24" t="str">
         <f t="shared" si="6"/>
@@ -13044,33 +13025,19 @@
       </c>
     </row>
     <row r="8" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="59">
-        <v>5</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G8" s="59">
-        <v>1</v>
-      </c>
-      <c r="H8" s="59">
-        <v>1</v>
-      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
       <c r="Q8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="R8" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" s="20">
         <f t="shared" si="2"/>
@@ -13078,7 +13045,7 @@
       </c>
       <c r="T8" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="20">
         <f t="shared" si="4"/>
@@ -13094,37 +13061,23 @@
       </c>
       <c r="Y8" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/LG</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="59">
-        <v>6</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="59">
-        <v>2</v>
-      </c>
-      <c r="H9" s="59">
-        <v>3</v>
-      </c>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
       <c r="Q9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="R9" s="19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S9" s="20">
         <f t="shared" si="2"/>
@@ -13136,7 +13089,7 @@
       </c>
       <c r="U9" s="20">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" s="24" t="str">
         <f t="shared" si="5"/>
@@ -13148,41 +13101,27 @@
       </c>
       <c r="Y9" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/WW</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="59">
-        <v>7</v>
-      </c>
-      <c r="C10" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="59">
-        <v>3</v>
-      </c>
-      <c r="H10" s="59">
-        <v>2</v>
-      </c>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
       <c r="Q10" s="3" t="s">
         <v>56</v>
       </c>
       <c r="R10" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="20">
         <f t="shared" si="3"/>
@@ -13202,37 +13141,23 @@
       </c>
       <c r="Y10" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/LG</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="59">
-        <v>8</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="59">
-        <v>4</v>
-      </c>
-      <c r="H11" s="59">
-        <v>4</v>
-      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
       <c r="Q11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="R11" s="19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S11" s="20">
         <f t="shared" si="2"/>
@@ -13240,7 +13165,7 @@
       </c>
       <c r="T11" s="20">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U11" s="20">
         <f t="shared" si="4"/>
@@ -13256,37 +13181,23 @@
       </c>
       <c r="Y11" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/WW</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="59">
-        <v>9</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G12" s="59">
-        <v>5</v>
-      </c>
-      <c r="H12" s="59">
-        <v>3</v>
-      </c>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
       <c r="Q12" s="3" t="s">
         <v>63</v>
       </c>
       <c r="R12" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="20">
         <f t="shared" si="2"/>
@@ -13294,7 +13205,7 @@
       </c>
       <c r="T12" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="20">
         <f t="shared" si="4"/>
@@ -13310,37 +13221,23 @@
       </c>
       <c r="Y12" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/LG</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="59">
-        <v>10</v>
-      </c>
-      <c r="C13" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G13" s="59">
-        <v>6</v>
-      </c>
-      <c r="H13" s="59">
-        <v>5</v>
-      </c>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
       <c r="Q13" s="3" t="s">
         <v>142</v>
       </c>
       <c r="R13" s="19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S13" s="20">
         <f t="shared" si="2"/>
@@ -13352,7 +13249,7 @@
       </c>
       <c r="U13" s="20">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13" s="24" t="str">
         <f t="shared" si="5"/>
@@ -13364,41 +13261,27 @@
       </c>
       <c r="Y13" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/WW</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="59">
-        <v>11</v>
-      </c>
-      <c r="C14" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="G14" s="59">
-        <v>7</v>
-      </c>
-      <c r="H14" s="59">
-        <v>4</v>
-      </c>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
       <c r="Q14" s="3" t="s">
         <v>148</v>
       </c>
       <c r="R14" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" s="20">
         <f t="shared" si="3"/>
@@ -13418,41 +13301,27 @@
       </c>
       <c r="Y14" s="24" t="str">
         <f t="shared" si="7"/>
-        <v>5M/LG</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="59">
-        <v>12</v>
-      </c>
-      <c r="C15" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" s="59">
-        <v>1</v>
-      </c>
-      <c r="H15" s="59">
-        <v>1</v>
-      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
       <c r="Q15" s="3" t="s">
         <v>72</v>
       </c>
       <c r="R15" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="20">
         <f t="shared" si="3"/>
@@ -13468,7 +13337,7 @@
       </c>
       <c r="X15" s="24" t="str">
         <f t="shared" si="6"/>
-        <v>WW/5M</v>
+        <v/>
       </c>
       <c r="Y15" s="24" t="str">
         <f t="shared" si="7"/>
@@ -13476,33 +13345,19 @@
       </c>
     </row>
     <row r="16" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="59">
-        <v>13</v>
-      </c>
-      <c r="C16" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" s="59">
-        <v>2</v>
-      </c>
-      <c r="H16" s="59">
-        <v>5</v>
-      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
       <c r="Q16" s="3" t="s">
         <v>76</v>
       </c>
       <c r="R16" s="19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S16" s="20">
         <f t="shared" si="2"/>
@@ -13514,7 +13369,7 @@
       </c>
       <c r="U16" s="20">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="24" t="str">
         <f t="shared" si="5"/>
@@ -13522,7 +13377,7 @@
       </c>
       <c r="X16" s="24" t="str">
         <f t="shared" si="6"/>
-        <v>WW/LG</v>
+        <v/>
       </c>
       <c r="Y16" s="24" t="str">
         <f t="shared" si="7"/>
@@ -13530,37 +13385,23 @@
       </c>
     </row>
     <row r="17" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="59">
-        <v>14</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="59" t="s">
-        <v>142</v>
-      </c>
-      <c r="F17" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G17" s="59">
-        <v>3</v>
-      </c>
-      <c r="H17" s="59">
-        <v>2</v>
-      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
       <c r="Q17" s="3" t="s">
         <v>79</v>
       </c>
       <c r="R17" s="19">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="20">
         <f t="shared" si="3"/>
@@ -13576,7 +13417,7 @@
       </c>
       <c r="X17" s="24" t="str">
         <f t="shared" si="6"/>
-        <v>WW/5M</v>
+        <v/>
       </c>
       <c r="Y17" s="24" t="str">
         <f t="shared" si="7"/>
@@ -13584,27 +13425,13 @@
       </c>
     </row>
     <row r="18" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="59">
-        <v>15</v>
-      </c>
-      <c r="C18" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="59">
-        <v>4</v>
-      </c>
-      <c r="H18" s="59">
-        <v>6</v>
-      </c>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
       <c r="S18" s="20"/>
       <c r="T18" s="20"/>
       <c r="U18" s="20"/>
@@ -13614,7 +13441,7 @@
       </c>
       <c r="X18" s="24" t="str">
         <f t="shared" si="6"/>
-        <v>WW/LG</v>
+        <v/>
       </c>
       <c r="Y18" s="24" t="str">
         <f t="shared" si="7"/>
@@ -13622,27 +13449,13 @@
       </c>
     </row>
     <row r="19" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="59">
-        <v>16</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G19" s="59">
-        <v>5</v>
-      </c>
-      <c r="H19" s="59">
-        <v>3</v>
-      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
       <c r="S19" s="20"/>
       <c r="T19" s="20"/>
       <c r="U19" s="20"/>
@@ -13652,7 +13465,7 @@
       </c>
       <c r="X19" s="24" t="str">
         <f t="shared" si="6"/>
-        <v>WW/5M</v>
+        <v/>
       </c>
       <c r="Y19" s="24" t="str">
         <f t="shared" si="7"/>
@@ -13789,7 +13602,7 @@
       </c>
       <c r="R26" s="19">
         <f t="shared" ref="R26:U26" si="8">R3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="19">
         <f t="shared" si="8"/>
@@ -13797,7 +13610,7 @@
       </c>
       <c r="T26" s="19">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="19">
         <f t="shared" si="8"/>
@@ -13824,7 +13637,7 @@
       <c r="I27" s="24"/>
       <c r="R27" s="19">
         <f t="shared" ref="R27:U27" si="9">R4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" s="19">
         <f t="shared" si="9"/>
@@ -13832,7 +13645,7 @@
       </c>
       <c r="T27" s="19">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27" s="19">
         <f t="shared" si="9"/>
@@ -13859,7 +13672,7 @@
       <c r="I28" s="24"/>
       <c r="R28" s="19">
         <f t="shared" ref="R28:U28" si="10">R5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S28" s="19">
         <f t="shared" si="10"/>
@@ -13871,7 +13684,7 @@
       </c>
       <c r="U28" s="19">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W28" s="24" t="str">
         <f t="shared" si="5"/>
@@ -13894,7 +13707,7 @@
       <c r="I29" s="24"/>
       <c r="R29" s="19">
         <f t="shared" ref="R29:U29" si="11">R6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S29" s="19">
         <f t="shared" si="11"/>
@@ -13906,7 +13719,7 @@
       </c>
       <c r="U29" s="19">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -13917,7 +13730,7 @@
       <c r="I30" s="24"/>
       <c r="R30" s="19">
         <f t="shared" ref="R30:U30" si="12">R7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30" s="19">
         <f t="shared" si="12"/>
@@ -13925,7 +13738,7 @@
       </c>
       <c r="T30" s="19">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U30" s="19">
         <f t="shared" si="12"/>
@@ -13935,7 +13748,7 @@
     <row r="31" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R31" s="19">
         <f t="shared" ref="R31:U31" si="13">R8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S31" s="19">
         <f t="shared" si="13"/>
@@ -13943,7 +13756,7 @@
       </c>
       <c r="T31" s="19">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U31" s="19">
         <f t="shared" si="13"/>
@@ -13953,7 +13766,7 @@
     <row r="32" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R32" s="19">
         <f t="shared" ref="R32:U32" si="14">R9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S32" s="19">
         <f t="shared" si="14"/>
@@ -13965,17 +13778,17 @@
       </c>
       <c r="U32" s="19">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R33" s="19">
         <f t="shared" ref="R33:U33" si="15">R10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" s="19">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T33" s="19">
         <f t="shared" si="15"/>
@@ -13989,7 +13802,7 @@
     <row r="34" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R34" s="19">
         <f t="shared" ref="R34:U34" si="16">R11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S34" s="19">
         <f t="shared" si="16"/>
@@ -13997,7 +13810,7 @@
       </c>
       <c r="T34" s="19">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U34" s="19">
         <f t="shared" si="16"/>
@@ -14007,7 +13820,7 @@
     <row r="35" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R35" s="19">
         <f t="shared" ref="R35:U35" si="17">R12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" s="19">
         <f t="shared" si="17"/>
@@ -14015,7 +13828,7 @@
       </c>
       <c r="T35" s="19">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U35" s="19">
         <f t="shared" si="17"/>
@@ -14025,7 +13838,7 @@
     <row r="36" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R36" s="19">
         <f t="shared" ref="R36:U36" si="18">R13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S36" s="19">
         <f t="shared" si="18"/>
@@ -14037,17 +13850,17 @@
       </c>
       <c r="U36" s="19">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R37" s="19">
         <f t="shared" ref="R37:U37" si="19">R14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" s="19">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="19">
         <f t="shared" si="19"/>
@@ -14061,11 +13874,11 @@
     <row r="38" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R38" s="19">
         <f t="shared" ref="R38:U38" si="20">R15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38" s="19">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T38" s="19">
         <f t="shared" si="20"/>
@@ -14079,7 +13892,7 @@
     <row r="39" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R39" s="19">
         <f t="shared" ref="R39:U39" si="21">R16</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S39" s="19">
         <f t="shared" si="21"/>
@@ -14091,17 +13904,17 @@
       </c>
       <c r="U39" s="19">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R40" s="19">
         <f t="shared" ref="R40:U40" si="22">R17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40" s="19">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T40" s="19">
         <f t="shared" si="22"/>
@@ -14109,6 +13922,2427 @@
       </c>
       <c r="U40" s="19">
         <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E7D6EA-0942-4896-8FCD-5B2FCE43B119}">
+  <dimension ref="B1:Y1000"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.73046875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="40" customWidth="1"/>
+    <col min="4" max="4" width="14" style="40" customWidth="1"/>
+    <col min="5" max="17" width="8.73046875" style="40" customWidth="1"/>
+    <col min="18" max="18" width="10.73046875" style="40" customWidth="1"/>
+    <col min="19" max="26" width="8.73046875" style="40" customWidth="1"/>
+    <col min="27" max="16384" width="14.3984375" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="24">
+        <f>COUNTIF(C3:C30, "Loose Gooses")</f>
+        <v>4</v>
+      </c>
+      <c r="M3" s="24">
+        <f>COUNTIF(D3:D30, "Loose Gooses")</f>
+        <v>6</v>
+      </c>
+      <c r="N3" s="23">
+        <f t="shared" ref="N3:N5" si="0">L3/(L3+M3)</f>
+        <v>0.4</v>
+      </c>
+      <c r="O3" s="24">
+        <f>IF(AND(N3&gt;N4, N3&gt;N5), 3, IF(OR(N3&gt;N4, N3&gt;N5), 2, 1))</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="19">
+        <f t="shared" ref="R3:R17" si="1">COUNTIF($E$3:$E$27, Q3)+U3</f>
+        <v>1</v>
+      </c>
+      <c r="S3" s="20">
+        <f t="shared" ref="S3:S17" si="2">COUNTIFS($E$3:$E$27, $Q3,$F$3:$F$27,"Finish")</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="20">
+        <f t="shared" ref="T3:T17" si="3">COUNTIFS($E$3:$E$27, $Q3,$F$3:$F$27,"Midrange")</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="20">
+        <f t="shared" ref="U3:U17" si="4">COUNTIFS($E$3:$E$27, $Q3,$F$3:$F$27,"Three Pointer")</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="59">
+        <v>1</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="59">
+        <v>1</v>
+      </c>
+      <c r="H4" s="59">
+        <v>1</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="24">
+        <f>COUNTIF(C3:C30, "5 Musketeers")</f>
+        <v>7</v>
+      </c>
+      <c r="M4" s="24">
+        <f>COUNTIF(D3:D30, "5 Musketeers")</f>
+        <v>5</v>
+      </c>
+      <c r="N4" s="23">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="O4" s="24">
+        <f>IF(AND(N4&gt;N3, N4&gt;N5), 3, IF(OR(N4&gt;N3, N4&gt;N5), 2, 1))</f>
+        <v>3</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S4" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U4" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="24" t="str">
+        <f>IF(AND(C4="Loose Gooses",D4="Wet Willies"),"LG/WW", IF(AND(C4="Loose Gooses",D4="5 Musketeers"),"LG/5M", ""))</f>
+        <v>LG/5M</v>
+      </c>
+      <c r="X4" s="24" t="str">
+        <f>IF(AND(C4="Wet Willies",D4="Loose Gooses"),"WW/LG", IF(AND(C4="Wet Willies",D4="5 Musketeers"),"WW/5M", ""))</f>
+        <v/>
+      </c>
+      <c r="Y4" s="24" t="str">
+        <f>IF(AND(C4="5 Musketeers",D4="Loose Gooses"),"5M/LG", IF(AND($C4="5 Musketeers",$D4="Wet Willies"),"5M/WW", ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="59">
+        <v>2</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="59">
+        <v>2</v>
+      </c>
+      <c r="H5" s="59">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="L5" s="24">
+        <f>COUNTIF(C3:C30, "Wet Willies")</f>
+        <v>5</v>
+      </c>
+      <c r="M5" s="24">
+        <f>COUNTIF(D3:D30, "Wet Willies")</f>
+        <v>5</v>
+      </c>
+      <c r="N5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="O5" s="24">
+        <f>IF(AND(N5&gt;N4, N5&gt;N3), 3, IF(OR(N5&gt;N4, N5&gt;N3), 2, 1))</f>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S5" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W5" s="24" t="str">
+        <f t="shared" ref="W5:W28" si="5">IF(AND(C5="Loose Gooses",D5="Wet Willies"),"LG/WW", IF(AND(C5="Loose Gooses",D5="5 Musketeers"),"LG/5M", ""))</f>
+        <v>LG/WW</v>
+      </c>
+      <c r="X5" s="24" t="str">
+        <f t="shared" ref="X5:X28" si="6">IF(AND(C5="Wet Willies",D5="Loose Gooses"),"WW/LG", IF(AND(C5="Wet Willies",D5="5 Musketeers"),"WW/5M", ""))</f>
+        <v/>
+      </c>
+      <c r="Y5" s="24" t="str">
+        <f t="shared" ref="Y5:Y28" si="7">IF(AND(C5="5 Musketeers",D5="Loose Gooses"),"5M/LG", IF(AND($C5="5 Musketeers",$D5="Wet Willies"),"5M/WW", ""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="59">
+        <v>3</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="59">
+        <v>3</v>
+      </c>
+      <c r="H6" s="59">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" s="19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W6" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>LG/5M</v>
+      </c>
+      <c r="X6" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y6" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="59">
+        <v>4</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="59">
+        <v>4</v>
+      </c>
+      <c r="H7" s="59">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S7" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U7" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>LG/WW</v>
+      </c>
+      <c r="X7" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y7" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="59">
+        <v>5</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="59">
+        <v>1</v>
+      </c>
+      <c r="H8" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S8" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U8" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X8" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y8" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/LG</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="59">
+        <v>6</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="59">
+        <v>2</v>
+      </c>
+      <c r="H9" s="59">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R9" s="19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W9" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X9" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y9" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/WW</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="59">
+        <v>7</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="59">
+        <v>3</v>
+      </c>
+      <c r="H10" s="59">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S10" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T10" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U10" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X10" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y10" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/LG</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="59">
+        <v>8</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="59">
+        <v>4</v>
+      </c>
+      <c r="H11" s="59">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S11" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="20">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U11" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X11" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y11" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/WW</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="59">
+        <v>9</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="59">
+        <v>5</v>
+      </c>
+      <c r="H12" s="59">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R12" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S12" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W12" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X12" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y12" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/LG</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="59">
+        <v>10</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="59">
+        <v>6</v>
+      </c>
+      <c r="H13" s="59">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="R13" s="19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S13" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W13" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X13" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y13" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/WW</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="59">
+        <v>11</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="59">
+        <v>7</v>
+      </c>
+      <c r="H14" s="59">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="R14" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S14" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T14" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X14" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y14" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v>5M/LG</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="59">
+        <v>12</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="59">
+        <v>1</v>
+      </c>
+      <c r="H15" s="59">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R15" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S15" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T15" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X15" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>WW/5M</v>
+      </c>
+      <c r="Y15" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="59">
+        <v>13</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" s="59">
+        <v>2</v>
+      </c>
+      <c r="H16" s="59">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R16" s="19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S16" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="20">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W16" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X16" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>WW/LG</v>
+      </c>
+      <c r="Y16" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="59">
+        <v>14</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="59">
+        <v>3</v>
+      </c>
+      <c r="H17" s="59">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R17" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S17" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T17" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W17" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X17" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>WW/5M</v>
+      </c>
+      <c r="Y17" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="59">
+        <v>15</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="59">
+        <v>4</v>
+      </c>
+      <c r="H18" s="59">
+        <v>6</v>
+      </c>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="W18" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X18" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>WW/LG</v>
+      </c>
+      <c r="Y18" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="59">
+        <v>16</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="59">
+        <v>5</v>
+      </c>
+      <c r="H19" s="59">
+        <v>3</v>
+      </c>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="W19" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X19" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v>WW/5M</v>
+      </c>
+      <c r="Y19" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W20" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X20" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y20" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W21" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X21" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y21" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W22" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X22" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y22" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="Q23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="W23" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X23" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y23" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E24" s="25"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="W24" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X24" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y24" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E25" s="25"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="Q25" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="R25" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="W25" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X25" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y25" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E26" s="25"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="Q26" s="26" t="str">
+        <f>C2</f>
+        <v>Insert Date Here</v>
+      </c>
+      <c r="R26" s="19">
+        <f t="shared" ref="R26:U40" si="8">R3</f>
+        <v>1</v>
+      </c>
+      <c r="S26" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="U26" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W26" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X26" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y26" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E27" s="25"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="R27" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S27" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="U27" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W27" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X27" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y27" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E28" s="25"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="R28" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S28" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U28" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="W28" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X28" s="24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y28" s="24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E29" s="25"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="R29" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S29" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E30" s="25"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="R30" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S30" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="U30" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R31" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S31" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="U31" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R32" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S32" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T32" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U32" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R33" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S33" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T33" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R34" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S34" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T34" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="U34" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R35" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S35" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T35" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="U35" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R36" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S36" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U36" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R37" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S37" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T37" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R38" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S38" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T38" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U38" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R39" s="19">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="S39" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="18:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="R40" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="S40" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T40" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="19">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>